<commit_message>
renamed bac bp go excel for gabrielle
</commit_message>
<xml_diff>
--- a/analyses/unipept/GO-terms/DN/TD+ND/dn80_bacteria_bioproc_GO.xlsx
+++ b/analyses/unipept/GO-terms/DN/TD+ND/dn80_bacteria_bioproc_GO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Raw GO counts DN80_combined_TD+" sheetId="1" state="visible" r:id="rId2"/>
@@ -3508,7 +3508,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3537,15 +3537,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3636,11 +3628,11 @@
   </sheetPr>
   <dimension ref="A1:E382"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A349" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C381" activeCellId="0" sqref="C381"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="97.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="9.78"/>
@@ -7826,7 +7818,7 @@
       <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.8"/>
@@ -19088,15 +19080,15 @@
   </sheetPr>
   <dimension ref="A1:J398"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="15.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.73"/>
@@ -19580,203 +19572,192 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7"/>
-      <c r="B32" s="8" t="s">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8" t="n">
+      <c r="C32" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="F32" s="8" t="n">
+      <c r="F32" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-    </row>
-    <row r="33" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7"/>
-      <c r="B33" s="8" t="s">
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="C33" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D33" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E33" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F33" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-    </row>
-    <row r="34" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7"/>
-      <c r="B34" s="8" t="s">
+      <c r="C33" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F33" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8" t="n">
+      <c r="C34" s="7"/>
+      <c r="D34" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="E34" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F34" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-    </row>
-    <row r="35" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7"/>
-      <c r="B35" s="8" t="s">
+      <c r="E34" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F34" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-    </row>
-    <row r="36" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7"/>
-      <c r="B36" s="8" t="s">
+      <c r="C35" s="7"/>
+      <c r="D35" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="E36" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F36" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-    </row>
-    <row r="37" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7"/>
-      <c r="B37" s="8" t="s">
+      <c r="C36" s="7"/>
+      <c r="D36" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E36" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F36" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-    </row>
-    <row r="38" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7"/>
-      <c r="B38" s="8" t="s">
+      <c r="C37" s="7"/>
+      <c r="D37" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E38" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-    </row>
-    <row r="39" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7"/>
-      <c r="B39" s="8" t="s">
+      <c r="C38" s="7"/>
+      <c r="D38" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-    </row>
-    <row r="40" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7"/>
-      <c r="B40" s="8" t="s">
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-    </row>
-    <row r="41" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="7"/>
-      <c r="B41" s="8" t="s">
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-    </row>
-    <row r="42" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="7"/>
-      <c r="B42" s="8" t="s">
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
     </row>
     <row r="43" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="s">
@@ -19815,59 +19796,56 @@
         <v>0.442477876106195</v>
       </c>
     </row>
-    <row r="44" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="7"/>
-      <c r="B44" s="8" t="s">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C44" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
-    </row>
-    <row r="45" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="7"/>
-      <c r="B45" s="8" t="s">
+      <c r="C44" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="8"/>
-    </row>
-    <row r="46" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="7"/>
-      <c r="B46" s="8" t="s">
+      <c r="C45" s="7"/>
+      <c r="D45" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E46" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F46" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="8"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E46" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F46" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
     </row>
     <row r="47" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="s">
@@ -19906,111 +19884,105 @@
         <v>1.76991150442478</v>
       </c>
     </row>
-    <row r="48" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="7"/>
-      <c r="B48" s="8" t="s">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C48" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
-    </row>
-    <row r="49" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="7"/>
-      <c r="B49" s="8" t="s">
+      <c r="C48" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="C49" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="8"/>
-    </row>
-    <row r="50" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="7"/>
-      <c r="B50" s="8" t="s">
+      <c r="C49" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C50" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="8"/>
-      <c r="J50" s="8"/>
-    </row>
-    <row r="51" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="7"/>
-      <c r="B51" s="8" t="s">
+      <c r="C50" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="8"/>
-      <c r="J51" s="8"/>
-    </row>
-    <row r="52" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="7"/>
-      <c r="B52" s="8" t="s">
+      <c r="C51" s="7"/>
+      <c r="D51" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="E52" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F52" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="G52" s="8"/>
-      <c r="H52" s="8"/>
-      <c r="I52" s="8"/>
-      <c r="J52" s="8"/>
-    </row>
-    <row r="53" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="7"/>
-      <c r="B53" s="8" t="s">
+      <c r="C52" s="7"/>
+      <c r="D52" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E52" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F52" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="7"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="E53" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F53" s="8" t="n">
+      <c r="C53" s="7"/>
+      <c r="D53" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E53" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F53" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="G53" s="8"/>
-      <c r="H53" s="8"/>
-      <c r="I53" s="8"/>
-      <c r="J53" s="8"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="7"/>
+      <c r="J53" s="7"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
@@ -20258,37 +20230,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="7"/>
-      <c r="B71" s="8" t="s">
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="C71" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D71" s="8"/>
-      <c r="E71" s="8"/>
-      <c r="F71" s="8"/>
-      <c r="G71" s="0"/>
-      <c r="H71" s="0"/>
-      <c r="I71" s="0"/>
-      <c r="J71" s="8"/>
-    </row>
-    <row r="72" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="7"/>
-      <c r="B72" s="8" t="s">
+      <c r="C71" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="J71" s="7"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="C72" s="8"/>
-      <c r="D72" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="E72" s="8"/>
-      <c r="F72" s="8"/>
-      <c r="G72" s="0"/>
-      <c r="H72" s="0"/>
-      <c r="I72" s="0"/>
-      <c r="J72" s="8"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
+      <c r="J72" s="7"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="0" t="s">
@@ -20399,77 +20363,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="7"/>
-      <c r="B84" s="8" t="s">
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="C84" s="8"/>
-      <c r="D84" s="8"/>
-      <c r="E84" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F84" s="8"/>
-      <c r="G84" s="8"/>
-      <c r="H84" s="8"/>
-      <c r="I84" s="8"/>
-      <c r="J84" s="8"/>
-    </row>
-    <row r="85" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="7"/>
-      <c r="B85" s="8" t="s">
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F84" s="7"/>
+      <c r="G84" s="7"/>
+      <c r="H84" s="7"/>
+      <c r="I84" s="7"/>
+      <c r="J84" s="7"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="C85" s="8"/>
-      <c r="D85" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E85" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F85" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G85" s="8"/>
-      <c r="H85" s="8"/>
-      <c r="I85" s="8"/>
-      <c r="J85" s="8"/>
-    </row>
-    <row r="86" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="7"/>
-      <c r="B86" s="8" t="s">
+      <c r="C85" s="7"/>
+      <c r="D85" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E85" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F85" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G85" s="7"/>
+      <c r="H85" s="7"/>
+      <c r="I85" s="7"/>
+      <c r="J85" s="7"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B86" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="C86" s="8"/>
-      <c r="D86" s="8"/>
-      <c r="E86" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F86" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G86" s="8"/>
-      <c r="H86" s="8"/>
-      <c r="I86" s="8"/>
-      <c r="J86" s="8"/>
-    </row>
-    <row r="87" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="7"/>
-      <c r="B87" s="8" t="s">
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F86" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G86" s="7"/>
+      <c r="H86" s="7"/>
+      <c r="I86" s="7"/>
+      <c r="J86" s="7"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B87" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="C87" s="8"/>
-      <c r="D87" s="8"/>
-      <c r="E87" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F87" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G87" s="8"/>
-      <c r="H87" s="8"/>
-      <c r="I87" s="8"/>
-      <c r="J87" s="8"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F87" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G87" s="7"/>
+      <c r="H87" s="7"/>
+      <c r="I87" s="7"/>
+      <c r="J87" s="7"/>
     </row>
     <row r="88" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="5" t="s">
@@ -22237,335 +22197,303 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="7"/>
-      <c r="B236" s="8" t="s">
+    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B236" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="C236" s="8"/>
-      <c r="D236" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="E236" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F236" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G236" s="0"/>
-      <c r="H236" s="0"/>
-      <c r="I236" s="0"/>
-      <c r="J236" s="8"/>
-    </row>
-    <row r="237" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="7"/>
-      <c r="B237" s="8" t="s">
+      <c r="C236" s="7"/>
+      <c r="D236" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E236" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F236" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J236" s="7"/>
+    </row>
+    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B237" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="C237" s="8"/>
-      <c r="D237" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="E237" s="8"/>
-      <c r="F237" s="8"/>
-      <c r="G237" s="0"/>
-      <c r="H237" s="0"/>
-      <c r="I237" s="0"/>
-      <c r="J237" s="8"/>
-    </row>
-    <row r="238" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A238" s="7"/>
-      <c r="B238" s="8" t="s">
+      <c r="C237" s="7"/>
+      <c r="D237" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E237" s="7"/>
+      <c r="F237" s="7"/>
+      <c r="J237" s="7"/>
+    </row>
+    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B238" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="C238" s="8"/>
-      <c r="D238" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E238" s="8"/>
-      <c r="F238" s="8"/>
-      <c r="G238" s="8"/>
-      <c r="H238" s="0"/>
-      <c r="I238" s="0"/>
-      <c r="J238" s="8"/>
-    </row>
-    <row r="239" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="7"/>
-      <c r="B239" s="8" t="s">
+      <c r="C238" s="7"/>
+      <c r="D238" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E238" s="7"/>
+      <c r="F238" s="7"/>
+      <c r="G238" s="7"/>
+      <c r="J238" s="7"/>
+    </row>
+    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B239" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="C239" s="8"/>
-      <c r="D239" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E239" s="8"/>
-      <c r="F239" s="8"/>
-      <c r="G239" s="8"/>
-      <c r="H239" s="8"/>
-      <c r="I239" s="0"/>
-      <c r="J239" s="8"/>
-    </row>
-    <row r="240" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="7"/>
-      <c r="B240" s="8" t="s">
+      <c r="C239" s="7"/>
+      <c r="D239" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E239" s="7"/>
+      <c r="F239" s="7"/>
+      <c r="G239" s="7"/>
+      <c r="H239" s="7"/>
+      <c r="J239" s="7"/>
+    </row>
+    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B240" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="C240" s="8"/>
-      <c r="D240" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E240" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F240" s="8"/>
-      <c r="G240" s="8"/>
-      <c r="H240" s="8"/>
-      <c r="I240" s="0"/>
-      <c r="J240" s="8"/>
-    </row>
-    <row r="241" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="7"/>
-      <c r="B241" s="8" t="s">
+      <c r="C240" s="7"/>
+      <c r="D240" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E240" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F240" s="7"/>
+      <c r="G240" s="7"/>
+      <c r="H240" s="7"/>
+      <c r="J240" s="7"/>
+    </row>
+    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B241" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="C241" s="8"/>
-      <c r="D241" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E241" s="8"/>
-      <c r="F241" s="8"/>
-      <c r="G241" s="8"/>
-      <c r="H241" s="8"/>
-      <c r="I241" s="0"/>
-      <c r="J241" s="8"/>
-    </row>
-    <row r="242" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="7"/>
-      <c r="B242" s="8" t="s">
+      <c r="C241" s="7"/>
+      <c r="D241" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E241" s="7"/>
+      <c r="F241" s="7"/>
+      <c r="G241" s="7"/>
+      <c r="H241" s="7"/>
+      <c r="J241" s="7"/>
+    </row>
+    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B242" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="C242" s="8"/>
-      <c r="D242" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E242" s="8"/>
-      <c r="F242" s="8"/>
-      <c r="G242" s="8"/>
-      <c r="H242" s="8"/>
-      <c r="I242" s="0"/>
-      <c r="J242" s="8"/>
-    </row>
-    <row r="243" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="7"/>
-      <c r="B243" s="8" t="s">
+      <c r="C242" s="7"/>
+      <c r="D242" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E242" s="7"/>
+      <c r="F242" s="7"/>
+      <c r="G242" s="7"/>
+      <c r="H242" s="7"/>
+      <c r="J242" s="7"/>
+    </row>
+    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B243" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="C243" s="8"/>
-      <c r="D243" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E243" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F243" s="8"/>
-      <c r="G243" s="8"/>
-      <c r="H243" s="8"/>
-      <c r="I243" s="8"/>
-      <c r="J243" s="8"/>
-    </row>
-    <row r="244" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="7"/>
-      <c r="B244" s="8" t="s">
+      <c r="C243" s="7"/>
+      <c r="D243" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E243" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F243" s="7"/>
+      <c r="G243" s="7"/>
+      <c r="H243" s="7"/>
+      <c r="I243" s="7"/>
+      <c r="J243" s="7"/>
+    </row>
+    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B244" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="C244" s="8"/>
-      <c r="D244" s="8"/>
-      <c r="E244" s="8" t="n">
+      <c r="C244" s="7"/>
+      <c r="D244" s="7"/>
+      <c r="E244" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="F244" s="8" t="n">
+      <c r="F244" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="G244" s="8"/>
-      <c r="H244" s="8"/>
-      <c r="I244" s="8"/>
-      <c r="J244" s="8"/>
-    </row>
-    <row r="245" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="7"/>
-      <c r="B245" s="8" t="s">
+      <c r="G244" s="7"/>
+      <c r="H244" s="7"/>
+      <c r="I244" s="7"/>
+      <c r="J244" s="7"/>
+    </row>
+    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B245" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="C245" s="8"/>
-      <c r="D245" s="8"/>
-      <c r="E245" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F245" s="8"/>
-      <c r="G245" s="8"/>
-      <c r="H245" s="8"/>
-      <c r="I245" s="8"/>
-      <c r="J245" s="8"/>
-    </row>
-    <row r="246" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A246" s="7"/>
-      <c r="B246" s="8" t="s">
+      <c r="C245" s="7"/>
+      <c r="D245" s="7"/>
+      <c r="E245" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F245" s="7"/>
+      <c r="G245" s="7"/>
+      <c r="H245" s="7"/>
+      <c r="I245" s="7"/>
+      <c r="J245" s="7"/>
+    </row>
+    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B246" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="C246" s="8"/>
-      <c r="D246" s="8"/>
-      <c r="E246" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F246" s="8"/>
-      <c r="G246" s="8"/>
-      <c r="H246" s="8"/>
-      <c r="I246" s="8"/>
-      <c r="J246" s="8"/>
-    </row>
-    <row r="247" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="7"/>
-      <c r="B247" s="8" t="s">
+      <c r="C246" s="7"/>
+      <c r="D246" s="7"/>
+      <c r="E246" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F246" s="7"/>
+      <c r="G246" s="7"/>
+      <c r="H246" s="7"/>
+      <c r="I246" s="7"/>
+      <c r="J246" s="7"/>
+    </row>
+    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B247" s="7" t="s">
         <v>308</v>
       </c>
-      <c r="C247" s="8"/>
-      <c r="D247" s="8"/>
-      <c r="E247" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F247" s="8"/>
-      <c r="G247" s="8"/>
-      <c r="H247" s="8"/>
-      <c r="I247" s="8"/>
-      <c r="J247" s="8"/>
-    </row>
-    <row r="248" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="7"/>
-      <c r="B248" s="8" t="s">
+      <c r="C247" s="7"/>
+      <c r="D247" s="7"/>
+      <c r="E247" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F247" s="7"/>
+      <c r="G247" s="7"/>
+      <c r="H247" s="7"/>
+      <c r="I247" s="7"/>
+      <c r="J247" s="7"/>
+    </row>
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B248" s="7" t="s">
         <v>334</v>
       </c>
-      <c r="C248" s="8"/>
-      <c r="D248" s="8"/>
-      <c r="E248" s="8"/>
-      <c r="F248" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G248" s="8"/>
-      <c r="H248" s="8"/>
-      <c r="I248" s="8"/>
-      <c r="J248" s="8"/>
-    </row>
-    <row r="249" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="7"/>
-      <c r="B249" s="8" t="s">
+      <c r="C248" s="7"/>
+      <c r="D248" s="7"/>
+      <c r="E248" s="7"/>
+      <c r="F248" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G248" s="7"/>
+      <c r="H248" s="7"/>
+      <c r="I248" s="7"/>
+      <c r="J248" s="7"/>
+    </row>
+    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B249" s="7" t="s">
         <v>347</v>
       </c>
-      <c r="C249" s="8"/>
-      <c r="D249" s="8"/>
-      <c r="E249" s="8"/>
-      <c r="F249" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G249" s="8"/>
-      <c r="H249" s="8"/>
-      <c r="I249" s="8"/>
-      <c r="J249" s="8"/>
-    </row>
-    <row r="250" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="7"/>
-      <c r="B250" s="8" t="s">
+      <c r="C249" s="7"/>
+      <c r="D249" s="7"/>
+      <c r="E249" s="7"/>
+      <c r="F249" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G249" s="7"/>
+      <c r="H249" s="7"/>
+      <c r="I249" s="7"/>
+      <c r="J249" s="7"/>
+    </row>
+    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B250" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="C250" s="8"/>
-      <c r="D250" s="8"/>
-      <c r="E250" s="8"/>
-      <c r="F250" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G250" s="8"/>
-      <c r="H250" s="8"/>
-      <c r="I250" s="8"/>
-      <c r="J250" s="8"/>
-    </row>
-    <row r="251" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="7"/>
-      <c r="B251" s="8" t="s">
+      <c r="C250" s="7"/>
+      <c r="D250" s="7"/>
+      <c r="E250" s="7"/>
+      <c r="F250" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G250" s="7"/>
+      <c r="H250" s="7"/>
+      <c r="I250" s="7"/>
+      <c r="J250" s="7"/>
+    </row>
+    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B251" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="C251" s="8"/>
-      <c r="D251" s="8"/>
-      <c r="E251" s="8"/>
-      <c r="F251" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G251" s="8"/>
-      <c r="H251" s="8"/>
-      <c r="I251" s="8"/>
-      <c r="J251" s="8"/>
-    </row>
-    <row r="252" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="7"/>
-      <c r="B252" s="8" t="s">
+      <c r="C251" s="7"/>
+      <c r="D251" s="7"/>
+      <c r="E251" s="7"/>
+      <c r="F251" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G251" s="7"/>
+      <c r="H251" s="7"/>
+      <c r="I251" s="7"/>
+      <c r="J251" s="7"/>
+    </row>
+    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B252" s="7" t="s">
         <v>362</v>
       </c>
-      <c r="C252" s="8"/>
-      <c r="D252" s="8"/>
-      <c r="E252" s="8"/>
-      <c r="F252" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G252" s="8"/>
-      <c r="H252" s="8"/>
-      <c r="I252" s="8"/>
-      <c r="J252" s="8"/>
-    </row>
-    <row r="253" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="7"/>
-      <c r="B253" s="8" t="s">
+      <c r="C252" s="7"/>
+      <c r="D252" s="7"/>
+      <c r="E252" s="7"/>
+      <c r="F252" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G252" s="7"/>
+      <c r="H252" s="7"/>
+      <c r="I252" s="7"/>
+      <c r="J252" s="7"/>
+    </row>
+    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B253" s="7" t="s">
         <v>365</v>
       </c>
-      <c r="C253" s="8"/>
-      <c r="D253" s="8"/>
-      <c r="E253" s="8"/>
-      <c r="F253" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G253" s="8"/>
-      <c r="H253" s="8"/>
-      <c r="I253" s="8"/>
-      <c r="J253" s="8"/>
-    </row>
-    <row r="254" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="7"/>
-      <c r="B254" s="8" t="s">
+      <c r="C253" s="7"/>
+      <c r="D253" s="7"/>
+      <c r="E253" s="7"/>
+      <c r="F253" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G253" s="7"/>
+      <c r="H253" s="7"/>
+      <c r="I253" s="7"/>
+      <c r="J253" s="7"/>
+    </row>
+    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B254" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="C254" s="8"/>
-      <c r="D254" s="8"/>
-      <c r="E254" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F254" s="8"/>
-      <c r="G254" s="8"/>
-      <c r="H254" s="8"/>
-      <c r="I254" s="8"/>
-      <c r="J254" s="8"/>
-    </row>
-    <row r="255" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="7"/>
-      <c r="B255" s="8" t="s">
+      <c r="C254" s="7"/>
+      <c r="D254" s="7"/>
+      <c r="E254" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F254" s="7"/>
+      <c r="G254" s="7"/>
+      <c r="H254" s="7"/>
+      <c r="I254" s="7"/>
+      <c r="J254" s="7"/>
+    </row>
+    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B255" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="C255" s="8"/>
-      <c r="D255" s="8"/>
-      <c r="E255" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F255" s="8"/>
-      <c r="G255" s="8"/>
-      <c r="H255" s="8"/>
-      <c r="I255" s="8"/>
-      <c r="J255" s="8"/>
+      <c r="C255" s="7"/>
+      <c r="D255" s="7"/>
+      <c r="E255" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F255" s="7"/>
+      <c r="G255" s="7"/>
+      <c r="H255" s="7"/>
+      <c r="I255" s="7"/>
+      <c r="J255" s="7"/>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B256" s="0" t="s">
@@ -22930,71 +22858,67 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="7"/>
-      <c r="B284" s="8" t="s">
+    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B284" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="C284" s="8"/>
-      <c r="D284" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E284" s="8"/>
-      <c r="F284" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G284" s="8"/>
-      <c r="H284" s="8"/>
-      <c r="I284" s="8"/>
-      <c r="J284" s="8"/>
-    </row>
-    <row r="285" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A285" s="7"/>
-      <c r="B285" s="8" t="s">
+      <c r="C284" s="7"/>
+      <c r="D284" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E284" s="7"/>
+      <c r="F284" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G284" s="7"/>
+      <c r="H284" s="7"/>
+      <c r="I284" s="7"/>
+      <c r="J284" s="7"/>
+    </row>
+    <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B285" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="C285" s="8"/>
-      <c r="D285" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E285" s="8"/>
-      <c r="F285" s="8"/>
-      <c r="G285" s="8"/>
-      <c r="H285" s="8"/>
-      <c r="I285" s="8"/>
-      <c r="J285" s="8"/>
-    </row>
-    <row r="286" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A286" s="7"/>
-      <c r="B286" s="8" t="s">
+      <c r="C285" s="7"/>
+      <c r="D285" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E285" s="7"/>
+      <c r="F285" s="7"/>
+      <c r="G285" s="7"/>
+      <c r="H285" s="7"/>
+      <c r="I285" s="7"/>
+      <c r="J285" s="7"/>
+    </row>
+    <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B286" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="C286" s="8"/>
-      <c r="D286" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E286" s="8"/>
-      <c r="F286" s="8"/>
-      <c r="G286" s="8"/>
-      <c r="H286" s="8"/>
-      <c r="I286" s="8"/>
-      <c r="J286" s="8"/>
-    </row>
-    <row r="287" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="7"/>
-      <c r="B287" s="8" t="s">
+      <c r="C286" s="7"/>
+      <c r="D286" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E286" s="7"/>
+      <c r="F286" s="7"/>
+      <c r="G286" s="7"/>
+      <c r="H286" s="7"/>
+      <c r="I286" s="7"/>
+      <c r="J286" s="7"/>
+    </row>
+    <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B287" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="C287" s="8"/>
-      <c r="D287" s="8"/>
-      <c r="E287" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F287" s="8"/>
-      <c r="G287" s="8"/>
-      <c r="H287" s="8"/>
-      <c r="I287" s="8"/>
-      <c r="J287" s="8"/>
+      <c r="C287" s="7"/>
+      <c r="D287" s="7"/>
+      <c r="E287" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F287" s="7"/>
+      <c r="G287" s="7"/>
+      <c r="H287" s="7"/>
+      <c r="I287" s="7"/>
+      <c r="J287" s="7"/>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B288" s="0" t="s">
@@ -23162,193 +23086,182 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A301" s="7"/>
-      <c r="B301" s="8" t="s">
+    <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B301" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="C301" s="8"/>
-      <c r="D301" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E301" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F301" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G301" s="8"/>
-      <c r="H301" s="8"/>
-      <c r="I301" s="8"/>
-      <c r="J301" s="8"/>
-    </row>
-    <row r="302" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A302" s="7"/>
-      <c r="B302" s="8" t="s">
+      <c r="C301" s="7"/>
+      <c r="D301" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E301" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F301" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G301" s="7"/>
+      <c r="H301" s="7"/>
+      <c r="I301" s="7"/>
+      <c r="J301" s="7"/>
+    </row>
+    <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B302" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="C302" s="8"/>
-      <c r="D302" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E302" s="8"/>
-      <c r="F302" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G302" s="8"/>
-      <c r="H302" s="8"/>
-      <c r="I302" s="8"/>
-      <c r="J302" s="8"/>
-    </row>
-    <row r="303" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A303" s="7"/>
-      <c r="B303" s="8" t="s">
+      <c r="C302" s="7"/>
+      <c r="D302" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E302" s="7"/>
+      <c r="F302" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G302" s="7"/>
+      <c r="H302" s="7"/>
+      <c r="I302" s="7"/>
+      <c r="J302" s="7"/>
+    </row>
+    <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B303" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="C303" s="8"/>
-      <c r="D303" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E303" s="8"/>
-      <c r="F303" s="8"/>
-      <c r="G303" s="8"/>
-      <c r="H303" s="8"/>
-      <c r="I303" s="8"/>
-      <c r="J303" s="8"/>
-    </row>
-    <row r="304" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A304" s="7"/>
-      <c r="B304" s="8" t="s">
+      <c r="C303" s="7"/>
+      <c r="D303" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E303" s="7"/>
+      <c r="F303" s="7"/>
+      <c r="G303" s="7"/>
+      <c r="H303" s="7"/>
+      <c r="I303" s="7"/>
+      <c r="J303" s="7"/>
+    </row>
+    <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B304" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="C304" s="8"/>
-      <c r="D304" s="8"/>
-      <c r="E304" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F304" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="G304" s="8"/>
-      <c r="H304" s="8"/>
-      <c r="I304" s="8"/>
-      <c r="J304" s="8"/>
-    </row>
-    <row r="305" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A305" s="7"/>
-      <c r="B305" s="8" t="s">
+      <c r="C304" s="7"/>
+      <c r="D304" s="7"/>
+      <c r="E304" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F304" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G304" s="7"/>
+      <c r="H304" s="7"/>
+      <c r="I304" s="7"/>
+      <c r="J304" s="7"/>
+    </row>
+    <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B305" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="C305" s="8"/>
-      <c r="D305" s="8"/>
-      <c r="E305" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F305" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G305" s="8"/>
-      <c r="H305" s="8"/>
-      <c r="I305" s="8"/>
-      <c r="J305" s="8"/>
-    </row>
-    <row r="306" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A306" s="7"/>
-      <c r="B306" s="8" t="s">
+      <c r="C305" s="7"/>
+      <c r="D305" s="7"/>
+      <c r="E305" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F305" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G305" s="7"/>
+      <c r="H305" s="7"/>
+      <c r="I305" s="7"/>
+      <c r="J305" s="7"/>
+    </row>
+    <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B306" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="C306" s="8"/>
-      <c r="D306" s="8"/>
-      <c r="E306" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F306" s="8"/>
-      <c r="G306" s="8"/>
-      <c r="H306" s="8"/>
-      <c r="I306" s="8"/>
-      <c r="J306" s="8"/>
-    </row>
-    <row r="307" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A307" s="7"/>
-      <c r="B307" s="8" t="s">
+      <c r="C306" s="7"/>
+      <c r="D306" s="7"/>
+      <c r="E306" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F306" s="7"/>
+      <c r="G306" s="7"/>
+      <c r="H306" s="7"/>
+      <c r="I306" s="7"/>
+      <c r="J306" s="7"/>
+    </row>
+    <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B307" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="C307" s="8"/>
-      <c r="D307" s="8"/>
-      <c r="E307" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F307" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G307" s="8"/>
-      <c r="H307" s="8"/>
-      <c r="I307" s="8"/>
-      <c r="J307" s="8"/>
-    </row>
-    <row r="308" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A308" s="7"/>
-      <c r="B308" s="8" t="s">
+      <c r="C307" s="7"/>
+      <c r="D307" s="7"/>
+      <c r="E307" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F307" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G307" s="7"/>
+      <c r="H307" s="7"/>
+      <c r="I307" s="7"/>
+      <c r="J307" s="7"/>
+    </row>
+    <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B308" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="C308" s="8"/>
-      <c r="D308" s="8"/>
-      <c r="E308" s="8"/>
-      <c r="F308" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="G308" s="8"/>
-      <c r="H308" s="8"/>
-      <c r="I308" s="8"/>
-      <c r="J308" s="8"/>
-    </row>
-    <row r="309" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A309" s="7"/>
-      <c r="B309" s="8" t="s">
+      <c r="C308" s="7"/>
+      <c r="D308" s="7"/>
+      <c r="E308" s="7"/>
+      <c r="F308" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G308" s="7"/>
+      <c r="H308" s="7"/>
+      <c r="I308" s="7"/>
+      <c r="J308" s="7"/>
+    </row>
+    <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B309" s="7" t="s">
         <v>331</v>
       </c>
-      <c r="C309" s="8"/>
-      <c r="D309" s="8"/>
-      <c r="E309" s="8"/>
-      <c r="F309" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G309" s="8"/>
-      <c r="H309" s="8"/>
-      <c r="I309" s="8"/>
-      <c r="J309" s="8"/>
-    </row>
-    <row r="310" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A310" s="7"/>
-      <c r="B310" s="8" t="s">
+      <c r="C309" s="7"/>
+      <c r="D309" s="7"/>
+      <c r="E309" s="7"/>
+      <c r="F309" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G309" s="7"/>
+      <c r="H309" s="7"/>
+      <c r="I309" s="7"/>
+      <c r="J309" s="7"/>
+    </row>
+    <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B310" s="7" t="s">
         <v>333</v>
       </c>
-      <c r="C310" s="8"/>
-      <c r="D310" s="8"/>
-      <c r="E310" s="8"/>
-      <c r="F310" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G310" s="8"/>
-      <c r="H310" s="8"/>
-      <c r="I310" s="8"/>
-      <c r="J310" s="8"/>
-    </row>
-    <row r="311" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A311" s="7"/>
-      <c r="B311" s="8" t="s">
+      <c r="C310" s="7"/>
+      <c r="D310" s="7"/>
+      <c r="E310" s="7"/>
+      <c r="F310" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G310" s="7"/>
+      <c r="H310" s="7"/>
+      <c r="I310" s="7"/>
+      <c r="J310" s="7"/>
+    </row>
+    <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B311" s="7" t="s">
         <v>345</v>
       </c>
-      <c r="C311" s="8"/>
-      <c r="D311" s="8"/>
-      <c r="E311" s="8"/>
-      <c r="F311" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G311" s="8"/>
-      <c r="H311" s="8"/>
-      <c r="I311" s="8"/>
-      <c r="J311" s="8"/>
+      <c r="C311" s="7"/>
+      <c r="D311" s="7"/>
+      <c r="E311" s="7"/>
+      <c r="F311" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G311" s="7"/>
+      <c r="H311" s="7"/>
+      <c r="I311" s="7"/>
+      <c r="J311" s="7"/>
     </row>
     <row r="312" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="5" t="s">
@@ -24252,23 +24165,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="389" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A389" s="10" t="s">
+    <row r="389" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A389" s="8" t="s">
         <v>1118</v>
       </c>
-      <c r="C389" s="11" t="n">
+      <c r="C389" s="9" t="n">
         <f aca="false">SUM(C2,C7,C13,C23,C29,C43,C47,C55,C88,C188,C198,C204,C213,C257,C261,C289,C312,C331,C339)</f>
         <v>302</v>
       </c>
-      <c r="D389" s="11" t="n">
+      <c r="D389" s="9" t="n">
         <f aca="false">SUM(D2,D7,D13,D23,D29,D43,D47,D55,D88,D188,D198,D204,D213,D257,D261,D289,D312,D331,D339)</f>
         <v>417</v>
       </c>
-      <c r="E389" s="11" t="n">
+      <c r="E389" s="9" t="n">
         <f aca="false">SUM(E2,E7,E13,E23,E29,E43,E47,E55,E88,E188,E198,E204,E213,E257,E261,E289,E312,E331,E339)</f>
         <v>304</v>
       </c>
-      <c r="F389" s="11" t="n">
+      <c r="F389" s="9" t="n">
         <f aca="false">SUM(F2,F7,F13,F23,F29,F43,F47,F55,F88,F188,F198,F204,F213,F257,F261,F289,F312,F331,F339)</f>
         <v>452</v>
       </c>
@@ -24402,7 +24315,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.94"/>
   </cols>
@@ -24792,11 +24705,11 @@
   </sheetPr>
   <dimension ref="A1:E218"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A75" activeCellId="0" sqref="A75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.98"/>
   </cols>

</xml_diff>